<commit_message>
productMenu: sort data by catagory & subCatagory front to back
</commit_message>
<xml_diff>
--- a/SurvivalGame/Assets/xlsxData/產品資料.xlsx
+++ b/SurvivalGame/Assets/xlsxData/產品資料.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\File\BS\Project\SurvivalGameWeb\SurvivalGame\SurvivalGame\Assets\xlsxData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\build_school\project\finalProject1\SurvivalGameVer2\SurvivalGame\Assets\xlsxData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="槍" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="364">
   <si>
     <t>名稱</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1355,10 +1355,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>null</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>585g</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1504,6 +1500,14 @@
   </si>
   <si>
     <t>ESS Profile Turbofan Goggles</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Standard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Standard</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1862,28 +1866,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="37.5" customWidth="1"/>
-    <col min="3" max="3" width="10.375" customWidth="1"/>
-    <col min="4" max="4" width="9.75" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
-    <col min="9" max="9" width="6.5" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="7.625" customWidth="1"/>
-    <col min="12" max="12" width="31.25" customWidth="1"/>
-    <col min="13" max="13" width="83.75" customWidth="1"/>
-    <col min="14" max="14" width="18.375" customWidth="1"/>
-    <col min="15" max="15" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" customWidth="1"/>
+    <col min="12" max="12" width="31.21875" customWidth="1"/>
+    <col min="13" max="13" width="83.77734375" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" customWidth="1"/>
+    <col min="15" max="15" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="22.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -1918,7 +1922,7 @@
         <v>7</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>13</v>
@@ -1930,7 +1934,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>38</v>
       </c>
@@ -1977,7 +1981,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="343.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="343.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
@@ -2024,7 +2028,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="189" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="244.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -2056,7 +2060,7 @@
         <v>35</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L4" s="2">
         <v>300</v>
@@ -2071,7 +2075,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="168" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="177.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
@@ -2118,12 +2122,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="315" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="377.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>55</v>
@@ -2165,12 +2169,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="273" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="355.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>55</v>
@@ -2212,7 +2216,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="273" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="355.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>76</v>
       </c>
@@ -2259,7 +2263,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="315" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="355.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>82</v>
       </c>
@@ -2306,7 +2310,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="231" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="288.60000000000002" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>83</v>
       </c>
@@ -2353,12 +2357,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>95</v>
@@ -2411,13 +2415,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="33.88671875" customWidth="1"/>
+    <col min="3" max="3" width="39.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2440,7 +2448,7 @@
         <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I1" t="s">
         <v>216</v>
@@ -2449,7 +2457,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>299</v>
       </c>
@@ -2481,12 +2489,12 @@
         <v>304</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C3" t="s">
         <v>305</v>
@@ -2513,12 +2521,12 @@
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C4" t="s">
         <v>305</v>
@@ -2545,7 +2553,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>312</v>
       </c>
@@ -2577,15 +2585,15 @@
         <v>317</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>318</v>
       </c>
       <c r="B6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>362</v>
       </c>
       <c r="D6" t="s">
         <v>319</v>
@@ -2609,7 +2617,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>323</v>
       </c>
@@ -2617,16 +2625,16 @@
         <v>324</v>
       </c>
       <c r="C7" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="D7" t="s">
         <v>217</v>
       </c>
       <c r="E7" t="s">
+        <v>325</v>
+      </c>
+      <c r="F7" t="s">
         <v>326</v>
-      </c>
-      <c r="F7" t="s">
-        <v>327</v>
       </c>
       <c r="G7" t="s">
         <v>303</v>
@@ -2638,18 +2646,18 @@
         <v>52</v>
       </c>
       <c r="J7" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D8" t="s">
         <v>217</v>
@@ -2658,7 +2666,7 @@
         <v>118</v>
       </c>
       <c r="F8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G8" t="s">
         <v>311</v>
@@ -2667,18 +2675,18 @@
         <v>54</v>
       </c>
       <c r="I8" t="s">
+        <v>329</v>
+      </c>
+      <c r="J8" t="s">
         <v>330</v>
       </c>
-      <c r="J8" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C9" t="s">
         <v>112</v>
@@ -2705,12 +2713,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>331</v>
+      </c>
+      <c r="B10" t="s">
         <v>332</v>
-      </c>
-      <c r="B10" t="s">
-        <v>333</v>
       </c>
       <c r="C10" t="s">
         <v>112</v>
@@ -2719,10 +2727,10 @@
         <v>32</v>
       </c>
       <c r="E10" t="s">
+        <v>333</v>
+      </c>
+      <c r="F10" t="s">
         <v>334</v>
-      </c>
-      <c r="F10" t="s">
-        <v>335</v>
       </c>
       <c r="G10" t="s">
         <v>33</v>
@@ -2731,18 +2739,18 @@
         <v>44</v>
       </c>
       <c r="I10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J10" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C11" t="s">
         <v>112</v>
@@ -2751,10 +2759,10 @@
         <v>32</v>
       </c>
       <c r="E11" t="s">
+        <v>337</v>
+      </c>
+      <c r="F11" t="s">
         <v>338</v>
-      </c>
-      <c r="F11" t="s">
-        <v>339</v>
       </c>
       <c r="G11" t="s">
         <v>33</v>
@@ -2772,6 +2780,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2783,14 +2792,14 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="56.125" customWidth="1"/>
-    <col min="4" max="4" width="10.375" customWidth="1"/>
-    <col min="5" max="5" width="13.875" customWidth="1"/>
+    <col min="2" max="2" width="56.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2810,7 +2819,7 @@
         <v>248</v>
       </c>
       <c r="G1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H1" t="s">
         <v>216</v>
@@ -2819,7 +2828,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>249</v>
       </c>
@@ -2848,7 +2857,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -2877,7 +2886,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>133</v>
       </c>
@@ -2906,7 +2915,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -2935,12 +2944,12 @@
         <v>222</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>262</v>
       </c>
       <c r="B6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C6" t="s">
         <v>223</v>
@@ -2964,7 +2973,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>138</v>
       </c>
@@ -2993,12 +3002,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>266</v>
       </c>
       <c r="B8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C8" t="s">
         <v>223</v>
@@ -3022,7 +3031,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>268</v>
       </c>
@@ -3051,12 +3060,12 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>142</v>
       </c>
       <c r="B10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C10" t="s">
         <v>223</v>
@@ -3080,7 +3089,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>144</v>
       </c>
@@ -3109,12 +3118,12 @@
         <v>254</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>145</v>
       </c>
       <c r="B12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C12" t="s">
         <v>233</v>
@@ -3138,7 +3147,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>146</v>
       </c>
@@ -3167,7 +3176,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>147</v>
       </c>
@@ -3196,7 +3205,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>148</v>
       </c>
@@ -3225,7 +3234,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>149</v>
       </c>
@@ -3254,7 +3263,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>150</v>
       </c>
@@ -3283,12 +3292,12 @@
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>151</v>
       </c>
       <c r="B18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C18" t="s">
         <v>233</v>
@@ -3312,7 +3321,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>152</v>
       </c>
@@ -3341,7 +3350,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>153</v>
       </c>
@@ -3370,7 +3379,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>154</v>
       </c>
@@ -3413,9 +3422,9 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3432,7 +3441,7 @@
         <v>110</v>
       </c>
       <c r="F1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G1" t="s">
         <v>157</v>
@@ -3441,12 +3450,12 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C2" t="s">
         <v>160</v>
@@ -3467,12 +3476,12 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C3" t="s">
         <v>160</v>
@@ -3493,7 +3502,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -3519,12 +3528,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>176</v>
       </c>
       <c r="B5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C5" t="s">
         <v>177</v>
@@ -3545,7 +3554,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>182</v>
       </c>
@@ -3571,7 +3580,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>188</v>
       </c>
@@ -3597,7 +3606,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="231" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="226.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>193</v>
       </c>
@@ -3623,12 +3632,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>199</v>
       </c>
       <c r="B9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C9" t="s">
         <v>200</v>
@@ -3649,12 +3658,12 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>204</v>
       </c>
       <c r="B10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C10" t="s">
         <v>205</v>
@@ -3672,7 +3681,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="264" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>209</v>
       </c>

</xml_diff>